<commit_message>
add new folder & calculate krippendorff's alpha.
</commit_message>
<xml_diff>
--- a/data/テンプレートアノテーション_20211020_整形後.xlsx
+++ b/data/テンプレートアノテーション_20211020_整形後.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shintaro/Documents/OPU/M12/exp_fb_cls/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D5250C6-BD79-6542-B3A9-FB53613A683A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C149BC-EDCA-B848-A2C6-A09AD7659A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -12306,7 +12305,7 @@
   <dimension ref="A1:P962"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>